<commit_message>
31.05.19 Today Sales Details 12:27 am
</commit_message>
<xml_diff>
--- a/May/Othes/Final Calculation of V48_skd and V92 for Price Adjustment_ BPA.XLSX
+++ b/May/Othes/Final Calculation of V48_skd and V92 for Price Adjustment_ BPA.XLSX
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
   </bookViews>
   <sheets>
     <sheet name="Final Summary" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Final Summary'!$A$8:$J$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Raw File'!$A$1:$F$84</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1063,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1480,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2633,8 +2633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>